<commit_message>
Correct input data bugs
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -29,7 +29,7 @@
     <definedName name="Region">'BAU Calculations'!$B$2</definedName>
     <definedName name="Unit.GW">[1]Conversions!$F$55</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2113,7 +2113,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3290,7 +3289,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6374,7 +6372,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11092,8 +11090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI103"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:AG62"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15028,6 +15026,1000 @@
         <v>1008970000000000</v>
       </c>
     </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A64" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C64" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D64" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E64" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F64" s="1">
+        <v>2022</v>
+      </c>
+      <c r="G64" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H64" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I64" s="1">
+        <v>2025</v>
+      </c>
+      <c r="J64" s="1">
+        <v>2026</v>
+      </c>
+      <c r="K64" s="1">
+        <v>2027</v>
+      </c>
+      <c r="L64" s="1">
+        <v>2028</v>
+      </c>
+      <c r="M64" s="1">
+        <v>2029</v>
+      </c>
+      <c r="N64" s="1">
+        <v>2030</v>
+      </c>
+      <c r="O64" s="1">
+        <v>2031</v>
+      </c>
+      <c r="P64" s="1">
+        <v>2032</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>2033</v>
+      </c>
+      <c r="R64" s="1">
+        <v>2034</v>
+      </c>
+      <c r="S64" s="1">
+        <v>2035</v>
+      </c>
+      <c r="T64" s="1">
+        <v>2036</v>
+      </c>
+      <c r="U64" s="1">
+        <v>2037</v>
+      </c>
+      <c r="V64" s="1">
+        <v>2038</v>
+      </c>
+      <c r="W64" s="1">
+        <v>2039</v>
+      </c>
+      <c r="X64" s="1">
+        <v>2040</v>
+      </c>
+      <c r="Y64" s="1">
+        <v>2041</v>
+      </c>
+      <c r="Z64" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AA64" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AB64" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AC64" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AD64" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AE64" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AF64" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AG64" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AH64" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A65" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="7">
+        <v>0</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0</v>
+      </c>
+      <c r="H65" s="7">
+        <v>0</v>
+      </c>
+      <c r="I65" s="7">
+        <v>0</v>
+      </c>
+      <c r="J65" s="7">
+        <v>0</v>
+      </c>
+      <c r="K65" s="7">
+        <v>0</v>
+      </c>
+      <c r="L65" s="7">
+        <v>0</v>
+      </c>
+      <c r="M65" s="7">
+        <v>0</v>
+      </c>
+      <c r="N65" s="7">
+        <v>0</v>
+      </c>
+      <c r="O65" s="7">
+        <v>0</v>
+      </c>
+      <c r="P65" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="7">
+        <v>0</v>
+      </c>
+      <c r="R65" s="7">
+        <v>0</v>
+      </c>
+      <c r="S65" s="7">
+        <v>0</v>
+      </c>
+      <c r="T65" s="7">
+        <v>0</v>
+      </c>
+      <c r="U65" s="7">
+        <v>0</v>
+      </c>
+      <c r="V65" s="7">
+        <v>0</v>
+      </c>
+      <c r="W65" s="7">
+        <v>0</v>
+      </c>
+      <c r="X65" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" cm="1">
+        <f t="array" ref="B66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,B64)</f>
+        <v>0</v>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" ref="D66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,D64)</f>
+        <v>1.1423612870660182E-3</v>
+      </c>
+      <c r="E66" cm="1">
+        <f t="array" ref="E66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,E64)</f>
+        <v>1.7135419305991384E-3</v>
+      </c>
+      <c r="F66" cm="1">
+        <f t="array" ref="F66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,F64)</f>
+        <v>2.2847225741322585E-3</v>
+      </c>
+      <c r="G66" cm="1">
+        <f t="array" ref="G66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,G64)</f>
+        <v>2.8559032176651566E-3</v>
+      </c>
+      <c r="H66" cm="1">
+        <f t="array" ref="H66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,H64)</f>
+        <v>3.4270838611982768E-3</v>
+      </c>
+      <c r="I66" cm="1">
+        <f t="array" ref="I66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,I64)</f>
+        <v>3.9982645047311749E-3</v>
+      </c>
+      <c r="J66" cm="1">
+        <f t="array" ref="J66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,J64)</f>
+        <v>4.569445148264295E-3</v>
+      </c>
+      <c r="K66" cm="1">
+        <f t="array" ref="K66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,K64)</f>
+        <v>5.1406257917974152E-3</v>
+      </c>
+      <c r="L66" cm="1">
+        <f t="array" ref="L66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,L64)</f>
+        <v>5.7118064353303133E-3</v>
+      </c>
+      <c r="M66" cm="1">
+        <f t="array" ref="M66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,M64)</f>
+        <v>6.2829870788634334E-3</v>
+      </c>
+      <c r="N66" cm="1">
+        <f t="array" ref="N66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,N64)</f>
+        <v>6.8541677223965536E-3</v>
+      </c>
+      <c r="O66" cm="1">
+        <f t="array" ref="O66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,O64)</f>
+        <v>7.4253483659294517E-3</v>
+      </c>
+      <c r="P66" cm="1">
+        <f t="array" ref="P66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,P64)</f>
+        <v>7.9965290094625718E-3</v>
+      </c>
+      <c r="Q66" cm="1">
+        <f t="array" ref="Q66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Q64)</f>
+        <v>8.5677096529954699E-3</v>
+      </c>
+      <c r="R66" cm="1">
+        <f t="array" ref="R66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,R64)</f>
+        <v>9.1388902965285901E-3</v>
+      </c>
+      <c r="S66" cm="1">
+        <f t="array" ref="S66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,S64)</f>
+        <v>9.7100709400617102E-3</v>
+      </c>
+      <c r="T66" cm="1">
+        <f t="array" ref="T66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,T64)</f>
+        <v>1.0281251583594608E-2</v>
+      </c>
+      <c r="U66" cm="1">
+        <f t="array" ref="U66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,U64)</f>
+        <v>1.0852432227127728E-2</v>
+      </c>
+      <c r="V66" cm="1">
+        <f t="array" ref="V66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,V64)</f>
+        <v>1.1423612870660849E-2</v>
+      </c>
+      <c r="W66" cm="1">
+        <f t="array" ref="W66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,W64)</f>
+        <v>1.1994793514193747E-2</v>
+      </c>
+      <c r="X66" cm="1">
+        <f t="array" ref="X66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,X64)</f>
+        <v>1.2565974157726867E-2</v>
+      </c>
+      <c r="Y66" cm="1">
+        <f t="array" ref="Y66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Y64)</f>
+        <v>1.3137154801259987E-2</v>
+      </c>
+      <c r="Z66" cm="1">
+        <f t="array" ref="Z66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Z64)</f>
+        <v>1.3708335444792885E-2</v>
+      </c>
+      <c r="AA66" cm="1">
+        <f t="array" ref="AA66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AA64)</f>
+        <v>1.4279516088326005E-2</v>
+      </c>
+      <c r="AB66" cm="1">
+        <f t="array" ref="AB66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AB64)</f>
+        <v>1.4850696731858903E-2</v>
+      </c>
+      <c r="AC66" cm="1">
+        <f t="array" ref="AC66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AC64)</f>
+        <v>1.5421877375392024E-2</v>
+      </c>
+      <c r="AD66" cm="1">
+        <f t="array" ref="AD66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AD64)</f>
+        <v>1.5993058018925144E-2</v>
+      </c>
+      <c r="AE66" cm="1">
+        <f t="array" ref="AE66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AE64)</f>
+        <v>1.6564238662458042E-2</v>
+      </c>
+      <c r="AF66" cm="1">
+        <f t="array" ref="AF66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AF64)</f>
+        <v>1.7135419305991162E-2</v>
+      </c>
+      <c r="AG66" cm="1">
+        <f t="array" ref="AG66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AG64)</f>
+        <v>1.7706599949524282E-2</v>
+      </c>
+      <c r="AH66" cm="1">
+        <f t="array" ref="AH66">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AH64)</f>
+        <v>1.827778059305718E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A67" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0</v>
+      </c>
+      <c r="H67" s="7">
+        <v>0</v>
+      </c>
+      <c r="I67" s="7">
+        <v>0</v>
+      </c>
+      <c r="J67" s="7">
+        <v>0</v>
+      </c>
+      <c r="K67" s="7">
+        <v>0</v>
+      </c>
+      <c r="L67" s="7">
+        <v>0</v>
+      </c>
+      <c r="M67" s="7">
+        <v>0</v>
+      </c>
+      <c r="N67" s="7">
+        <v>0</v>
+      </c>
+      <c r="O67" s="7">
+        <v>0</v>
+      </c>
+      <c r="P67" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>0</v>
+      </c>
+      <c r="R67" s="7">
+        <v>0</v>
+      </c>
+      <c r="S67" s="7">
+        <v>0</v>
+      </c>
+      <c r="T67" s="7">
+        <v>0</v>
+      </c>
+      <c r="U67" s="7">
+        <v>0</v>
+      </c>
+      <c r="V67" s="7">
+        <v>0</v>
+      </c>
+      <c r="W67" s="7">
+        <v>0</v>
+      </c>
+      <c r="X67" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A68" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="7">
+        <v>0</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0</v>
+      </c>
+      <c r="G68" s="7">
+        <v>0</v>
+      </c>
+      <c r="H68" s="7">
+        <v>0</v>
+      </c>
+      <c r="I68" s="7">
+        <v>0</v>
+      </c>
+      <c r="J68" s="7">
+        <v>0</v>
+      </c>
+      <c r="K68" s="7">
+        <v>0</v>
+      </c>
+      <c r="L68" s="7">
+        <v>0</v>
+      </c>
+      <c r="M68" s="7">
+        <v>0</v>
+      </c>
+      <c r="N68" s="7">
+        <v>0</v>
+      </c>
+      <c r="O68" s="7">
+        <v>0</v>
+      </c>
+      <c r="P68" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="7">
+        <v>0</v>
+      </c>
+      <c r="R68" s="7">
+        <v>0</v>
+      </c>
+      <c r="S68" s="7">
+        <v>0</v>
+      </c>
+      <c r="T68" s="7">
+        <v>0</v>
+      </c>
+      <c r="U68" s="7">
+        <v>0</v>
+      </c>
+      <c r="V68" s="7">
+        <v>0</v>
+      </c>
+      <c r="W68" s="7">
+        <v>0</v>
+      </c>
+      <c r="X68" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" cm="1">
+        <f t="array" ref="B69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,B64)</f>
+        <v>0</v>
+      </c>
+      <c r="D69" cm="1">
+        <f t="array" ref="D69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,D64)</f>
+        <v>8.355507555716235E-4</v>
+      </c>
+      <c r="E69" cm="1">
+        <f t="array" ref="E69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,E64)</f>
+        <v>1.2533261333574908E-3</v>
+      </c>
+      <c r="F69" cm="1">
+        <f t="array" ref="F69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,F64)</f>
+        <v>1.671101511143358E-3</v>
+      </c>
+      <c r="G69" cm="1">
+        <f t="array" ref="G69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,G64)</f>
+        <v>2.0888768889291143E-3</v>
+      </c>
+      <c r="H69" cm="1">
+        <f t="array" ref="H69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,H64)</f>
+        <v>2.5066522667149815E-3</v>
+      </c>
+      <c r="I69" cm="1">
+        <f t="array" ref="I69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,I64)</f>
+        <v>2.9244276445007378E-3</v>
+      </c>
+      <c r="J69" cm="1">
+        <f t="array" ref="J69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,J64)</f>
+        <v>3.342203022286605E-3</v>
+      </c>
+      <c r="K69" cm="1">
+        <f t="array" ref="K69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,K64)</f>
+        <v>3.7599784000723613E-3</v>
+      </c>
+      <c r="L69" cm="1">
+        <f t="array" ref="L69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,L64)</f>
+        <v>4.1777537778582285E-3</v>
+      </c>
+      <c r="M69" cm="1">
+        <f t="array" ref="M69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,M64)</f>
+        <v>4.5955291556439848E-3</v>
+      </c>
+      <c r="N69" cm="1">
+        <f t="array" ref="N69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,N64)</f>
+        <v>5.0133045334298521E-3</v>
+      </c>
+      <c r="O69" cm="1">
+        <f t="array" ref="O69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,O64)</f>
+        <v>5.4310799112157193E-3</v>
+      </c>
+      <c r="P69" cm="1">
+        <f t="array" ref="P69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,P64)</f>
+        <v>5.8488552890014756E-3</v>
+      </c>
+      <c r="Q69" cm="1">
+        <f t="array" ref="Q69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Q64)</f>
+        <v>6.2666306667873428E-3</v>
+      </c>
+      <c r="R69" cm="1">
+        <f t="array" ref="R69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,R64)</f>
+        <v>6.6844060445730991E-3</v>
+      </c>
+      <c r="S69" cm="1">
+        <f t="array" ref="S69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,S64)</f>
+        <v>7.1021814223589663E-3</v>
+      </c>
+      <c r="T69" cm="1">
+        <f t="array" ref="T69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,T64)</f>
+        <v>7.5199568001447226E-3</v>
+      </c>
+      <c r="U69" cm="1">
+        <f t="array" ref="U69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,U64)</f>
+        <v>7.9377321779305898E-3</v>
+      </c>
+      <c r="V69" cm="1">
+        <f t="array" ref="V69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,V64)</f>
+        <v>8.3555075557163461E-3</v>
+      </c>
+      <c r="W69" cm="1">
+        <f t="array" ref="W69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,W64)</f>
+        <v>8.7732829335022133E-3</v>
+      </c>
+      <c r="X69" cm="1">
+        <f t="array" ref="X69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,X64)</f>
+        <v>9.1910583112880806E-3</v>
+      </c>
+      <c r="Y69" cm="1">
+        <f t="array" ref="Y69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Y64)</f>
+        <v>9.6088336890738368E-3</v>
+      </c>
+      <c r="Z69" cm="1">
+        <f t="array" ref="Z69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Z64)</f>
+        <v>1.0026609066859704E-2</v>
+      </c>
+      <c r="AA69" cm="1">
+        <f t="array" ref="AA69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AA64)</f>
+        <v>1.044438444464546E-2</v>
+      </c>
+      <c r="AB69" cm="1">
+        <f t="array" ref="AB69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AB64)</f>
+        <v>1.0862159822431328E-2</v>
+      </c>
+      <c r="AC69" cm="1">
+        <f t="array" ref="AC69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AC64)</f>
+        <v>1.1279935200217084E-2</v>
+      </c>
+      <c r="AD69" cm="1">
+        <f t="array" ref="AD69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AD64)</f>
+        <v>1.1697710578002951E-2</v>
+      </c>
+      <c r="AE69" cm="1">
+        <f t="array" ref="AE69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AE64)</f>
+        <v>1.2115485955788707E-2</v>
+      </c>
+      <c r="AF69" cm="1">
+        <f t="array" ref="AF69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AF64)</f>
+        <v>1.2533261333574575E-2</v>
+      </c>
+      <c r="AG69" cm="1">
+        <f t="array" ref="AG69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AG64)</f>
+        <v>1.2951036711360442E-2</v>
+      </c>
+      <c r="AH69" cm="1">
+        <f t="array" ref="AH69">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AH64)</f>
+        <v>1.3368812089146198E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A70" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="7">
+        <v>0</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0</v>
+      </c>
+      <c r="D70" s="7">
+        <v>0</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0</v>
+      </c>
+      <c r="F70" s="7">
+        <v>0</v>
+      </c>
+      <c r="G70" s="7">
+        <v>0</v>
+      </c>
+      <c r="H70" s="7">
+        <v>0</v>
+      </c>
+      <c r="I70" s="7">
+        <v>0</v>
+      </c>
+      <c r="J70" s="7">
+        <v>0</v>
+      </c>
+      <c r="K70" s="7">
+        <v>0</v>
+      </c>
+      <c r="L70" s="7">
+        <v>0</v>
+      </c>
+      <c r="M70" s="7">
+        <v>0</v>
+      </c>
+      <c r="N70" s="7">
+        <v>0</v>
+      </c>
+      <c r="O70" s="7">
+        <v>0</v>
+      </c>
+      <c r="P70" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="7">
+        <v>0</v>
+      </c>
+      <c r="R70" s="7">
+        <v>0</v>
+      </c>
+      <c r="S70" s="7">
+        <v>0</v>
+      </c>
+      <c r="T70" s="7">
+        <v>0</v>
+      </c>
+      <c r="U70" s="7">
+        <v>0</v>
+      </c>
+      <c r="V70" s="7">
+        <v>0</v>
+      </c>
+      <c r="W70" s="7">
+        <v>0</v>
+      </c>
+      <c r="X70" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y70" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG70" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH70" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="7">
+        <v>0</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0</v>
+      </c>
+      <c r="H71" s="7">
+        <v>0</v>
+      </c>
+      <c r="I71" s="7">
+        <v>0</v>
+      </c>
+      <c r="J71" s="7">
+        <v>0</v>
+      </c>
+      <c r="K71" s="7">
+        <v>0</v>
+      </c>
+      <c r="L71" s="7">
+        <v>0</v>
+      </c>
+      <c r="M71" s="7">
+        <v>0</v>
+      </c>
+      <c r="N71" s="7">
+        <v>0</v>
+      </c>
+      <c r="O71" s="7">
+        <v>0</v>
+      </c>
+      <c r="P71" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="7">
+        <v>0</v>
+      </c>
+      <c r="R71" s="7">
+        <v>0</v>
+      </c>
+      <c r="S71" s="7">
+        <v>0</v>
+      </c>
+      <c r="T71" s="7">
+        <v>0</v>
+      </c>
+      <c r="U71" s="7">
+        <v>0</v>
+      </c>
+      <c r="V71" s="7">
+        <v>0</v>
+      </c>
+      <c r="W71" s="7">
+        <v>0</v>
+      </c>
+      <c r="X71" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y71" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG71" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:34" x14ac:dyDescent="0.45">
+      <c r="A72" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="7">
+        <v>0</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0</v>
+      </c>
+      <c r="D72" s="7">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0</v>
+      </c>
+      <c r="G72" s="7">
+        <v>0</v>
+      </c>
+      <c r="H72" s="7">
+        <v>0</v>
+      </c>
+      <c r="I72" s="7">
+        <v>0</v>
+      </c>
+      <c r="J72" s="7">
+        <v>0</v>
+      </c>
+      <c r="K72" s="7">
+        <v>0</v>
+      </c>
+      <c r="L72" s="7">
+        <v>0</v>
+      </c>
+      <c r="M72" s="7">
+        <v>0</v>
+      </c>
+      <c r="N72" s="7">
+        <v>0</v>
+      </c>
+      <c r="O72" s="7">
+        <v>0</v>
+      </c>
+      <c r="P72" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="7">
+        <v>0</v>
+      </c>
+      <c r="R72" s="7">
+        <v>0</v>
+      </c>
+      <c r="S72" s="7">
+        <v>0</v>
+      </c>
+      <c r="T72" s="7">
+        <v>0</v>
+      </c>
+      <c r="U72" s="7">
+        <v>0</v>
+      </c>
+      <c r="V72" s="7">
+        <v>0</v>
+      </c>
+      <c r="W72" s="7">
+        <v>0</v>
+      </c>
+      <c r="X72" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG72" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="7">
+        <v>0</v>
+      </c>
+    </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" s="15" t="s">
         <v>120</v>
@@ -15498,10 +16490,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15615,131 +16607,131 @@
         <v>221</v>
       </c>
       <c r="B2" cm="1">
-        <f t="array" ref="B2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,C39)</f>
+        <f t="array" ref="B2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!C64)</f>
         <v>5.7118064353312015E-4</v>
       </c>
       <c r="C2" cm="1">
-        <f t="array" ref="C2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,D39)</f>
+        <f t="array" ref="C2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!D64)</f>
         <v>1.1423612870660182E-3</v>
       </c>
       <c r="D2" cm="1">
-        <f t="array" ref="D2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,E39)</f>
+        <f t="array" ref="D2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!E64)</f>
         <v>1.7135419305991384E-3</v>
       </c>
       <c r="E2" cm="1">
-        <f t="array" ref="E2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,F39)</f>
+        <f t="array" ref="E2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!F64)</f>
         <v>2.2847225741322585E-3</v>
       </c>
       <c r="F2" cm="1">
-        <f t="array" ref="F2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,G39)</f>
+        <f t="array" ref="F2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!G64)</f>
         <v>2.8559032176651566E-3</v>
       </c>
       <c r="G2" cm="1">
-        <f t="array" ref="G2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,H39)</f>
+        <f t="array" ref="G2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!H64)</f>
         <v>3.4270838611982768E-3</v>
       </c>
       <c r="H2" cm="1">
-        <f t="array" ref="H2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,I39)</f>
+        <f t="array" ref="H2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!I64)</f>
         <v>3.9982645047311749E-3</v>
       </c>
       <c r="I2" cm="1">
-        <f t="array" ref="I2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,J39)</f>
+        <f t="array" ref="I2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!J64)</f>
         <v>4.569445148264295E-3</v>
       </c>
       <c r="J2" cm="1">
-        <f t="array" ref="J2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,K39)</f>
+        <f t="array" ref="J2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!K64)</f>
         <v>5.1406257917974152E-3</v>
       </c>
       <c r="K2" cm="1">
-        <f t="array" ref="K2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,L39)</f>
+        <f t="array" ref="K2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!L64)</f>
         <v>5.7118064353303133E-3</v>
       </c>
       <c r="L2" cm="1">
-        <f t="array" ref="L2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,M39)</f>
+        <f t="array" ref="L2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!M64)</f>
         <v>6.2829870788634334E-3</v>
       </c>
       <c r="M2" cm="1">
-        <f t="array" ref="M2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,N39)</f>
+        <f t="array" ref="M2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!N64)</f>
         <v>6.8541677223965536E-3</v>
       </c>
       <c r="N2" cm="1">
-        <f t="array" ref="N2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,O39)</f>
+        <f t="array" ref="N2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!O64)</f>
         <v>7.4253483659294517E-3</v>
       </c>
       <c r="O2" cm="1">
-        <f t="array" ref="O2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,P39)</f>
+        <f t="array" ref="O2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!P64)</f>
         <v>7.9965290094625718E-3</v>
       </c>
       <c r="P2" cm="1">
-        <f t="array" ref="P2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Q39)</f>
+        <f t="array" ref="P2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!Q64)</f>
         <v>8.5677096529954699E-3</v>
       </c>
       <c r="Q2" cm="1">
-        <f t="array" ref="Q2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,R39)</f>
+        <f t="array" ref="Q2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!R64)</f>
         <v>9.1388902965285901E-3</v>
       </c>
       <c r="R2" cm="1">
-        <f t="array" ref="R2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,S39)</f>
+        <f t="array" ref="R2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!S64)</f>
         <v>9.7100709400617102E-3</v>
       </c>
       <c r="S2" cm="1">
-        <f t="array" ref="S2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,T39)</f>
+        <f t="array" ref="S2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!T64)</f>
         <v>1.0281251583594608E-2</v>
       </c>
       <c r="T2" cm="1">
-        <f t="array" ref="T2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,U39)</f>
+        <f t="array" ref="T2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!U64)</f>
         <v>1.0852432227127728E-2</v>
       </c>
       <c r="U2" cm="1">
-        <f t="array" ref="U2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,V39)</f>
+        <f t="array" ref="U2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!V64)</f>
         <v>1.1423612870660849E-2</v>
       </c>
       <c r="V2" cm="1">
-        <f t="array" ref="V2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,W39)</f>
+        <f t="array" ref="V2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!W64)</f>
         <v>1.1994793514193747E-2</v>
       </c>
       <c r="W2" cm="1">
-        <f t="array" ref="W2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,X39)</f>
+        <f t="array" ref="W2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!X64)</f>
         <v>1.2565974157726867E-2</v>
       </c>
       <c r="X2" cm="1">
-        <f t="array" ref="X2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Y39)</f>
+        <f t="array" ref="X2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!Y64)</f>
         <v>1.3137154801259987E-2</v>
       </c>
       <c r="Y2" cm="1">
-        <f t="array" ref="Y2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Z39)</f>
+        <f t="array" ref="Y2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!Z64)</f>
         <v>1.3708335444792885E-2</v>
       </c>
       <c r="Z2" cm="1">
-        <f t="array" ref="Z2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AA39)</f>
+        <f t="array" ref="Z2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AA64)</f>
         <v>1.4279516088326005E-2</v>
       </c>
       <c r="AA2" cm="1">
-        <f t="array" ref="AA2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AB39)</f>
+        <f t="array" ref="AA2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AB64)</f>
         <v>1.4850696731858903E-2</v>
       </c>
       <c r="AB2" cm="1">
-        <f t="array" ref="AB2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AC39)</f>
+        <f t="array" ref="AB2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AC64)</f>
         <v>1.5421877375392024E-2</v>
       </c>
       <c r="AC2" cm="1">
-        <f t="array" ref="AC2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AD39)</f>
+        <f t="array" ref="AC2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AD64)</f>
         <v>1.5993058018925144E-2</v>
       </c>
       <c r="AD2" cm="1">
-        <f t="array" ref="AD2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AE39)</f>
+        <f t="array" ref="AD2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AE64)</f>
         <v>1.6564238662458042E-2</v>
       </c>
       <c r="AE2" cm="1">
-        <f t="array" ref="AE2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AF39)</f>
+        <f t="array" ref="AE2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AF64)</f>
         <v>1.7135419305991162E-2</v>
       </c>
       <c r="AF2" cm="1">
-        <f t="array" ref="AF2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AG39)</f>
+        <f t="array" ref="AF2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AG64)</f>
         <v>1.7706599949524282E-2</v>
       </c>
       <c r="AG2" cm="1">
-        <f t="array" ref="AG2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AH39)</f>
+        <f t="array" ref="AG2">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,'BAU Calculations'!AH64)</f>
         <v>1.827778059305718E-2</v>
       </c>
     </row>
@@ -17255,1000 +18247,6 @@
         <v>0</v>
       </c>
       <c r="AG17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="1">
-        <v>2018</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2019</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E39" s="1">
-        <v>2021</v>
-      </c>
-      <c r="F39" s="1">
-        <v>2022</v>
-      </c>
-      <c r="G39" s="1">
-        <v>2023</v>
-      </c>
-      <c r="H39" s="1">
-        <v>2024</v>
-      </c>
-      <c r="I39" s="1">
-        <v>2025</v>
-      </c>
-      <c r="J39" s="1">
-        <v>2026</v>
-      </c>
-      <c r="K39" s="1">
-        <v>2027</v>
-      </c>
-      <c r="L39" s="1">
-        <v>2028</v>
-      </c>
-      <c r="M39" s="1">
-        <v>2029</v>
-      </c>
-      <c r="N39" s="1">
-        <v>2030</v>
-      </c>
-      <c r="O39" s="1">
-        <v>2031</v>
-      </c>
-      <c r="P39" s="1">
-        <v>2032</v>
-      </c>
-      <c r="Q39" s="1">
-        <v>2033</v>
-      </c>
-      <c r="R39" s="1">
-        <v>2034</v>
-      </c>
-      <c r="S39" s="1">
-        <v>2035</v>
-      </c>
-      <c r="T39" s="1">
-        <v>2036</v>
-      </c>
-      <c r="U39" s="1">
-        <v>2037</v>
-      </c>
-      <c r="V39" s="1">
-        <v>2038</v>
-      </c>
-      <c r="W39" s="1">
-        <v>2039</v>
-      </c>
-      <c r="X39" s="1">
-        <v>2040</v>
-      </c>
-      <c r="Y39" s="1">
-        <v>2041</v>
-      </c>
-      <c r="Z39" s="1">
-        <v>2042</v>
-      </c>
-      <c r="AA39" s="1">
-        <v>2043</v>
-      </c>
-      <c r="AB39" s="1">
-        <v>2044</v>
-      </c>
-      <c r="AC39" s="1">
-        <v>2045</v>
-      </c>
-      <c r="AD39" s="1">
-        <v>2046</v>
-      </c>
-      <c r="AE39" s="1">
-        <v>2047</v>
-      </c>
-      <c r="AF39" s="1">
-        <v>2048</v>
-      </c>
-      <c r="AG39" s="1">
-        <v>2049</v>
-      </c>
-      <c r="AH39" s="1">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A40" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="7">
-        <v>0</v>
-      </c>
-      <c r="C40" s="7">
-        <v>0</v>
-      </c>
-      <c r="D40" s="7">
-        <v>0</v>
-      </c>
-      <c r="E40" s="7">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7">
-        <v>0</v>
-      </c>
-      <c r="G40" s="7">
-        <v>0</v>
-      </c>
-      <c r="H40" s="7">
-        <v>0</v>
-      </c>
-      <c r="I40" s="7">
-        <v>0</v>
-      </c>
-      <c r="J40" s="7">
-        <v>0</v>
-      </c>
-      <c r="K40" s="7">
-        <v>0</v>
-      </c>
-      <c r="L40" s="7">
-        <v>0</v>
-      </c>
-      <c r="M40" s="7">
-        <v>0</v>
-      </c>
-      <c r="N40" s="7">
-        <v>0</v>
-      </c>
-      <c r="O40" s="7">
-        <v>0</v>
-      </c>
-      <c r="P40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="7">
-        <v>0</v>
-      </c>
-      <c r="R40" s="7">
-        <v>0</v>
-      </c>
-      <c r="S40" s="7">
-        <v>0</v>
-      </c>
-      <c r="T40" s="7">
-        <v>0</v>
-      </c>
-      <c r="U40" s="7">
-        <v>0</v>
-      </c>
-      <c r="V40" s="7">
-        <v>0</v>
-      </c>
-      <c r="W40" s="7">
-        <v>0</v>
-      </c>
-      <c r="X40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG40" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" cm="1">
-        <f t="array" ref="B41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,B39)</f>
-        <v>0</v>
-      </c>
-      <c r="D41" cm="1">
-        <f t="array" ref="D41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,D39)</f>
-        <v>1.1423612870660182E-3</v>
-      </c>
-      <c r="E41" cm="1">
-        <f t="array" ref="E41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,E39)</f>
-        <v>1.7135419305991384E-3</v>
-      </c>
-      <c r="F41" cm="1">
-        <f t="array" ref="F41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,F39)</f>
-        <v>2.2847225741322585E-3</v>
-      </c>
-      <c r="G41" cm="1">
-        <f t="array" ref="G41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,G39)</f>
-        <v>2.8559032176651566E-3</v>
-      </c>
-      <c r="H41" cm="1">
-        <f t="array" ref="H41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,H39)</f>
-        <v>3.4270838611982768E-3</v>
-      </c>
-      <c r="I41" cm="1">
-        <f t="array" ref="I41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,I39)</f>
-        <v>3.9982645047311749E-3</v>
-      </c>
-      <c r="J41" cm="1">
-        <f t="array" ref="J41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,J39)</f>
-        <v>4.569445148264295E-3</v>
-      </c>
-      <c r="K41" cm="1">
-        <f t="array" ref="K41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,K39)</f>
-        <v>5.1406257917974152E-3</v>
-      </c>
-      <c r="L41" cm="1">
-        <f t="array" ref="L41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,L39)</f>
-        <v>5.7118064353303133E-3</v>
-      </c>
-      <c r="M41" cm="1">
-        <f t="array" ref="M41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,M39)</f>
-        <v>6.2829870788634334E-3</v>
-      </c>
-      <c r="N41" cm="1">
-        <f t="array" ref="N41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,N39)</f>
-        <v>6.8541677223965536E-3</v>
-      </c>
-      <c r="O41" cm="1">
-        <f t="array" ref="O41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,O39)</f>
-        <v>7.4253483659294517E-3</v>
-      </c>
-      <c r="P41" cm="1">
-        <f t="array" ref="P41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,P39)</f>
-        <v>7.9965290094625718E-3</v>
-      </c>
-      <c r="Q41" cm="1">
-        <f t="array" ref="Q41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Q39)</f>
-        <v>8.5677096529954699E-3</v>
-      </c>
-      <c r="R41" cm="1">
-        <f t="array" ref="R41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,R39)</f>
-        <v>9.1388902965285901E-3</v>
-      </c>
-      <c r="S41" cm="1">
-        <f t="array" ref="S41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,S39)</f>
-        <v>9.7100709400617102E-3</v>
-      </c>
-      <c r="T41" cm="1">
-        <f t="array" ref="T41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,T39)</f>
-        <v>1.0281251583594608E-2</v>
-      </c>
-      <c r="U41" cm="1">
-        <f t="array" ref="U41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,U39)</f>
-        <v>1.0852432227127728E-2</v>
-      </c>
-      <c r="V41" cm="1">
-        <f t="array" ref="V41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,V39)</f>
-        <v>1.1423612870660849E-2</v>
-      </c>
-      <c r="W41" cm="1">
-        <f t="array" ref="W41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,W39)</f>
-        <v>1.1994793514193747E-2</v>
-      </c>
-      <c r="X41" cm="1">
-        <f t="array" ref="X41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,X39)</f>
-        <v>1.2565974157726867E-2</v>
-      </c>
-      <c r="Y41" cm="1">
-        <f t="array" ref="Y41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Y39)</f>
-        <v>1.3137154801259987E-2</v>
-      </c>
-      <c r="Z41" cm="1">
-        <f t="array" ref="Z41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,Z39)</f>
-        <v>1.3708335444792885E-2</v>
-      </c>
-      <c r="AA41" cm="1">
-        <f t="array" ref="AA41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AA39)</f>
-        <v>1.4279516088326005E-2</v>
-      </c>
-      <c r="AB41" cm="1">
-        <f t="array" ref="AB41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AB39)</f>
-        <v>1.4850696731858903E-2</v>
-      </c>
-      <c r="AC41" cm="1">
-        <f t="array" ref="AC41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AC39)</f>
-        <v>1.5421877375392024E-2</v>
-      </c>
-      <c r="AD41" cm="1">
-        <f t="array" ref="AD41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AD39)</f>
-        <v>1.5993058018925144E-2</v>
-      </c>
-      <c r="AE41" cm="1">
-        <f t="array" ref="AE41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AE39)</f>
-        <v>1.6564238662458042E-2</v>
-      </c>
-      <c r="AF41" cm="1">
-        <f t="array" ref="AF41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AF39)</f>
-        <v>1.7135419305991162E-2</v>
-      </c>
-      <c r="AG41" cm="1">
-        <f t="array" ref="AG41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AG39)</f>
-        <v>1.7706599949524282E-2</v>
-      </c>
-      <c r="AH41" cm="1">
-        <f t="array" ref="AH41">TREND('BAU Calculations'!$B102:$C102,'BAU Calculations'!$B101:$C101,AH39)</f>
-        <v>1.827778059305718E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A42" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="7">
-        <v>0</v>
-      </c>
-      <c r="C42" s="7">
-        <v>0</v>
-      </c>
-      <c r="D42" s="7">
-        <v>0</v>
-      </c>
-      <c r="E42" s="7">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7">
-        <v>0</v>
-      </c>
-      <c r="G42" s="7">
-        <v>0</v>
-      </c>
-      <c r="H42" s="7">
-        <v>0</v>
-      </c>
-      <c r="I42" s="7">
-        <v>0</v>
-      </c>
-      <c r="J42" s="7">
-        <v>0</v>
-      </c>
-      <c r="K42" s="7">
-        <v>0</v>
-      </c>
-      <c r="L42" s="7">
-        <v>0</v>
-      </c>
-      <c r="M42" s="7">
-        <v>0</v>
-      </c>
-      <c r="N42" s="7">
-        <v>0</v>
-      </c>
-      <c r="O42" s="7">
-        <v>0</v>
-      </c>
-      <c r="P42" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="7">
-        <v>0</v>
-      </c>
-      <c r="R42" s="7">
-        <v>0</v>
-      </c>
-      <c r="S42" s="7">
-        <v>0</v>
-      </c>
-      <c r="T42" s="7">
-        <v>0</v>
-      </c>
-      <c r="U42" s="7">
-        <v>0</v>
-      </c>
-      <c r="V42" s="7">
-        <v>0</v>
-      </c>
-      <c r="W42" s="7">
-        <v>0</v>
-      </c>
-      <c r="X42" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG42" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A43" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="7">
-        <v>0</v>
-      </c>
-      <c r="C43" s="7">
-        <v>0</v>
-      </c>
-      <c r="D43" s="7">
-        <v>0</v>
-      </c>
-      <c r="E43" s="7">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7">
-        <v>0</v>
-      </c>
-      <c r="G43" s="7">
-        <v>0</v>
-      </c>
-      <c r="H43" s="7">
-        <v>0</v>
-      </c>
-      <c r="I43" s="7">
-        <v>0</v>
-      </c>
-      <c r="J43" s="7">
-        <v>0</v>
-      </c>
-      <c r="K43" s="7">
-        <v>0</v>
-      </c>
-      <c r="L43" s="7">
-        <v>0</v>
-      </c>
-      <c r="M43" s="7">
-        <v>0</v>
-      </c>
-      <c r="N43" s="7">
-        <v>0</v>
-      </c>
-      <c r="O43" s="7">
-        <v>0</v>
-      </c>
-      <c r="P43" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="7">
-        <v>0</v>
-      </c>
-      <c r="R43" s="7">
-        <v>0</v>
-      </c>
-      <c r="S43" s="7">
-        <v>0</v>
-      </c>
-      <c r="T43" s="7">
-        <v>0</v>
-      </c>
-      <c r="U43" s="7">
-        <v>0</v>
-      </c>
-      <c r="V43" s="7">
-        <v>0</v>
-      </c>
-      <c r="W43" s="7">
-        <v>0</v>
-      </c>
-      <c r="X43" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG43" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" cm="1">
-        <f t="array" ref="B44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,B39)</f>
-        <v>0</v>
-      </c>
-      <c r="D44" cm="1">
-        <f t="array" ref="D44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,D39)</f>
-        <v>8.355507555716235E-4</v>
-      </c>
-      <c r="E44" cm="1">
-        <f t="array" ref="E44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,E39)</f>
-        <v>1.2533261333574908E-3</v>
-      </c>
-      <c r="F44" cm="1">
-        <f t="array" ref="F44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,F39)</f>
-        <v>1.671101511143358E-3</v>
-      </c>
-      <c r="G44" cm="1">
-        <f t="array" ref="G44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,G39)</f>
-        <v>2.0888768889291143E-3</v>
-      </c>
-      <c r="H44" cm="1">
-        <f t="array" ref="H44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,H39)</f>
-        <v>2.5066522667149815E-3</v>
-      </c>
-      <c r="I44" cm="1">
-        <f t="array" ref="I44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,I39)</f>
-        <v>2.9244276445007378E-3</v>
-      </c>
-      <c r="J44" cm="1">
-        <f t="array" ref="J44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,J39)</f>
-        <v>3.342203022286605E-3</v>
-      </c>
-      <c r="K44" cm="1">
-        <f t="array" ref="K44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,K39)</f>
-        <v>3.7599784000723613E-3</v>
-      </c>
-      <c r="L44" cm="1">
-        <f t="array" ref="L44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,L39)</f>
-        <v>4.1777537778582285E-3</v>
-      </c>
-      <c r="M44" cm="1">
-        <f t="array" ref="M44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,M39)</f>
-        <v>4.5955291556439848E-3</v>
-      </c>
-      <c r="N44" cm="1">
-        <f t="array" ref="N44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,N39)</f>
-        <v>5.0133045334298521E-3</v>
-      </c>
-      <c r="O44" cm="1">
-        <f t="array" ref="O44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,O39)</f>
-        <v>5.4310799112157193E-3</v>
-      </c>
-      <c r="P44" cm="1">
-        <f t="array" ref="P44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,P39)</f>
-        <v>5.8488552890014756E-3</v>
-      </c>
-      <c r="Q44" cm="1">
-        <f t="array" ref="Q44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Q39)</f>
-        <v>6.2666306667873428E-3</v>
-      </c>
-      <c r="R44" cm="1">
-        <f t="array" ref="R44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,R39)</f>
-        <v>6.6844060445730991E-3</v>
-      </c>
-      <c r="S44" cm="1">
-        <f t="array" ref="S44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,S39)</f>
-        <v>7.1021814223589663E-3</v>
-      </c>
-      <c r="T44" cm="1">
-        <f t="array" ref="T44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,T39)</f>
-        <v>7.5199568001447226E-3</v>
-      </c>
-      <c r="U44" cm="1">
-        <f t="array" ref="U44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,U39)</f>
-        <v>7.9377321779305898E-3</v>
-      </c>
-      <c r="V44" cm="1">
-        <f t="array" ref="V44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,V39)</f>
-        <v>8.3555075557163461E-3</v>
-      </c>
-      <c r="W44" cm="1">
-        <f t="array" ref="W44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,W39)</f>
-        <v>8.7732829335022133E-3</v>
-      </c>
-      <c r="X44" cm="1">
-        <f t="array" ref="X44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,X39)</f>
-        <v>9.1910583112880806E-3</v>
-      </c>
-      <c r="Y44" cm="1">
-        <f t="array" ref="Y44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Y39)</f>
-        <v>9.6088336890738368E-3</v>
-      </c>
-      <c r="Z44" cm="1">
-        <f t="array" ref="Z44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,Z39)</f>
-        <v>1.0026609066859704E-2</v>
-      </c>
-      <c r="AA44" cm="1">
-        <f t="array" ref="AA44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AA39)</f>
-        <v>1.044438444464546E-2</v>
-      </c>
-      <c r="AB44" cm="1">
-        <f t="array" ref="AB44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AB39)</f>
-        <v>1.0862159822431328E-2</v>
-      </c>
-      <c r="AC44" cm="1">
-        <f t="array" ref="AC44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AC39)</f>
-        <v>1.1279935200217084E-2</v>
-      </c>
-      <c r="AD44" cm="1">
-        <f t="array" ref="AD44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AD39)</f>
-        <v>1.1697710578002951E-2</v>
-      </c>
-      <c r="AE44" cm="1">
-        <f t="array" ref="AE44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AE39)</f>
-        <v>1.2115485955788707E-2</v>
-      </c>
-      <c r="AF44" cm="1">
-        <f t="array" ref="AF44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AF39)</f>
-        <v>1.2533261333574575E-2</v>
-      </c>
-      <c r="AG44" cm="1">
-        <f t="array" ref="AG44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AG39)</f>
-        <v>1.2951036711360442E-2</v>
-      </c>
-      <c r="AH44" cm="1">
-        <f t="array" ref="AH44">TREND('BAU Calculations'!$B103:$C103,'BAU Calculations'!$B101:$C101,AH39)</f>
-        <v>1.3368812089146198E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A45" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="7">
-        <v>0</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0</v>
-      </c>
-      <c r="D45" s="7">
-        <v>0</v>
-      </c>
-      <c r="E45" s="7">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7">
-        <v>0</v>
-      </c>
-      <c r="G45" s="7">
-        <v>0</v>
-      </c>
-      <c r="H45" s="7">
-        <v>0</v>
-      </c>
-      <c r="I45" s="7">
-        <v>0</v>
-      </c>
-      <c r="J45" s="7">
-        <v>0</v>
-      </c>
-      <c r="K45" s="7">
-        <v>0</v>
-      </c>
-      <c r="L45" s="7">
-        <v>0</v>
-      </c>
-      <c r="M45" s="7">
-        <v>0</v>
-      </c>
-      <c r="N45" s="7">
-        <v>0</v>
-      </c>
-      <c r="O45" s="7">
-        <v>0</v>
-      </c>
-      <c r="P45" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="7">
-        <v>0</v>
-      </c>
-      <c r="R45" s="7">
-        <v>0</v>
-      </c>
-      <c r="S45" s="7">
-        <v>0</v>
-      </c>
-      <c r="T45" s="7">
-        <v>0</v>
-      </c>
-      <c r="U45" s="7">
-        <v>0</v>
-      </c>
-      <c r="V45" s="7">
-        <v>0</v>
-      </c>
-      <c r="W45" s="7">
-        <v>0</v>
-      </c>
-      <c r="X45" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG45" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH45" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A46" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="7">
-        <v>0</v>
-      </c>
-      <c r="C46" s="7">
-        <v>0</v>
-      </c>
-      <c r="D46" s="7">
-        <v>0</v>
-      </c>
-      <c r="E46" s="7">
-        <v>0</v>
-      </c>
-      <c r="F46" s="7">
-        <v>0</v>
-      </c>
-      <c r="G46" s="7">
-        <v>0</v>
-      </c>
-      <c r="H46" s="7">
-        <v>0</v>
-      </c>
-      <c r="I46" s="7">
-        <v>0</v>
-      </c>
-      <c r="J46" s="7">
-        <v>0</v>
-      </c>
-      <c r="K46" s="7">
-        <v>0</v>
-      </c>
-      <c r="L46" s="7">
-        <v>0</v>
-      </c>
-      <c r="M46" s="7">
-        <v>0</v>
-      </c>
-      <c r="N46" s="7">
-        <v>0</v>
-      </c>
-      <c r="O46" s="7">
-        <v>0</v>
-      </c>
-      <c r="P46" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="7">
-        <v>0</v>
-      </c>
-      <c r="R46" s="7">
-        <v>0</v>
-      </c>
-      <c r="S46" s="7">
-        <v>0</v>
-      </c>
-      <c r="T46" s="7">
-        <v>0</v>
-      </c>
-      <c r="U46" s="7">
-        <v>0</v>
-      </c>
-      <c r="V46" s="7">
-        <v>0</v>
-      </c>
-      <c r="W46" s="7">
-        <v>0</v>
-      </c>
-      <c r="X46" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG46" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH46" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
-      <c r="A47" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="7">
-        <v>0</v>
-      </c>
-      <c r="C47" s="7">
-        <v>0</v>
-      </c>
-      <c r="D47" s="7">
-        <v>0</v>
-      </c>
-      <c r="E47" s="7">
-        <v>0</v>
-      </c>
-      <c r="F47" s="7">
-        <v>0</v>
-      </c>
-      <c r="G47" s="7">
-        <v>0</v>
-      </c>
-      <c r="H47" s="7">
-        <v>0</v>
-      </c>
-      <c r="I47" s="7">
-        <v>0</v>
-      </c>
-      <c r="J47" s="7">
-        <v>0</v>
-      </c>
-      <c r="K47" s="7">
-        <v>0</v>
-      </c>
-      <c r="L47" s="7">
-        <v>0</v>
-      </c>
-      <c r="M47" s="7">
-        <v>0</v>
-      </c>
-      <c r="N47" s="7">
-        <v>0</v>
-      </c>
-      <c r="O47" s="7">
-        <v>0</v>
-      </c>
-      <c r="P47" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="7">
-        <v>0</v>
-      </c>
-      <c r="R47" s="7">
-        <v>0</v>
-      </c>
-      <c r="S47" s="7">
-        <v>0</v>
-      </c>
-      <c r="T47" s="7">
-        <v>0</v>
-      </c>
-      <c r="U47" s="7">
-        <v>0</v>
-      </c>
-      <c r="V47" s="7">
-        <v>0</v>
-      </c>
-      <c r="W47" s="7">
-        <v>0</v>
-      </c>
-      <c r="X47" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG47" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH47" s="7">
         <v>0</v>
       </c>
     </row>
@@ -18265,8 +18263,8 @@
   </sheetPr>
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:AG9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18379,6 +18377,9 @@
       <c r="A2" s="54" t="s">
         <v>187</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>

</xml_diff>